<commit_message>
add user name to availability booking table, new seed, redirect external type only
</commit_message>
<xml_diff>
--- a/prisma/data/data-users.xlsx
+++ b/prisma/data/data-users.xlsx
@@ -53,7 +53,7 @@
     <t>Manager Unit</t>
   </si>
   <si>
-    <t>habib.muhajir99@gmail.com</t>
+    <t>habib.muhajir@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>WAHYOE ROBBYANUR</t>
@@ -65,7 +65,7 @@
     <t>K3 &amp; Keamanan</t>
   </si>
   <si>
-    <t>Wahyoerobbyanur@gmail.com</t>
+    <t>wahyoe.robbyanur@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>ANGGA SENJA PRASETYA</t>
@@ -74,7 +74,7 @@
     <t>9116070TB</t>
   </si>
   <si>
-    <t>Anggasenja30@gmail.com</t>
+    <t>9116070TB@pln-npservices.com</t>
   </si>
   <si>
     <t>DENI PURWOWISESO</t>
@@ -167,7 +167,7 @@
     <t>Lingkungan</t>
   </si>
   <si>
-    <t>B.crisviandi@gmail.com</t>
+    <t>bhekty.crisviandi@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>ANDI AYU WILDANA</t>
@@ -176,7 +176,7 @@
     <t>9317002TB</t>
   </si>
   <si>
-    <t>Ayuwildana@gmail.com</t>
+    <t>9317002TB@pln-npservices.com</t>
   </si>
   <si>
     <t>KOKOH WAHYU ADILLAH</t>
@@ -185,7 +185,7 @@
     <t>9014056RB</t>
   </si>
   <si>
-    <t>kokoh.adillah@gmail.com</t>
+    <t>9014056RB@pln-npservices.com</t>
   </si>
   <si>
     <t>JUMADI</t>
@@ -233,7 +233,7 @@
     <t>Operasi</t>
   </si>
   <si>
-    <t>Dhi2k10@gmail.com</t>
+    <t>dhidhik.krido@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>DIDIK AGUS SETIAWAN</t>
@@ -245,7 +245,7 @@
     <t>Rendal Operasi</t>
   </si>
   <si>
-    <t>setiawandidikagus@gmail.com</t>
+    <t>didik.agus@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>LUMBAN GAOL CRISTOFEL</t>
@@ -254,7 +254,7 @@
     <t>9316036TB</t>
   </si>
   <si>
-    <t>lumbancris@gmail.com</t>
+    <t>9316036TB@pln-npservices.com</t>
   </si>
   <si>
     <t>RAMSES HASUDUNGAN SIMATUPANG</t>
@@ -263,7 +263,7 @@
     <t>9016067TB</t>
   </si>
   <si>
-    <t>Ramcs.okm@gmail.com</t>
+    <t>9016067TB@pln-npservices.com</t>
   </si>
   <si>
     <t>ADITYA KUMARA TUNGGA</t>
@@ -272,7 +272,7 @@
     <t>9616046TB</t>
   </si>
   <si>
-    <t>Adityakumara76@gmail.com</t>
+    <t>9616046TB@pln-npservices.com</t>
   </si>
   <si>
     <t>HERI FALENTINO</t>
@@ -293,7 +293,7 @@
     <t>Produksi A</t>
   </si>
   <si>
-    <t>andi_istrada@yahoo.com</t>
+    <t>andi.istrada@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>ADI HERLAMBANG</t>
@@ -302,7 +302,7 @@
     <t>9116014TB</t>
   </si>
   <si>
-    <t>Adihrlmbng@gmail.com</t>
+    <t>9116014TB@pln-npservices.com</t>
   </si>
   <si>
     <t>ARDIKA RIO NINDRA</t>
@@ -311,7 +311,7 @@
     <t>9216051TB</t>
   </si>
   <si>
-    <t>Dikario.b4k3uniba13@gmail.com</t>
+    <t>9216051TB@pln-npservices.com</t>
   </si>
   <si>
     <t>NANDA FINALIS</t>
@@ -320,7 +320,7 @@
     <t>9016022TB</t>
   </si>
   <si>
-    <t>Nandafinalis@gmail.com</t>
+    <t>9016022TB@pln-npservices.com</t>
   </si>
   <si>
     <t>RAHMANSYAH</t>
@@ -329,7 +329,7 @@
     <t>9216010TB</t>
   </si>
   <si>
-    <t>rahman.ujkt@gmail.com</t>
+    <t>9216010TB@pln-npservices.com</t>
   </si>
   <si>
     <t>SIGIT HARIYAWAN</t>
@@ -338,7 +338,7 @@
     <t>9616048TB</t>
   </si>
   <si>
-    <t>Sigithariyawan@gmail.com</t>
+    <t>9616048TB@pln-npservices.com</t>
   </si>
   <si>
     <t>KSATRIAWAN DWIGUNA</t>
@@ -347,7 +347,7 @@
     <t>9316044TB</t>
   </si>
   <si>
-    <t>Ksatriawan22@gmail.com</t>
+    <t>9316044TB@pln-npservices.com</t>
   </si>
   <si>
     <t>MUHAMMAD RIZAL PERDANA</t>
@@ -356,7 +356,7 @@
     <t>9216119TB</t>
   </si>
   <si>
-    <t>Rperdana400@gmail.com</t>
+    <t>9216119TB@pln-npservices.com</t>
   </si>
   <si>
     <t>LUKI DWI ARGO SAPUTRO</t>
@@ -365,7 +365,7 @@
     <t>9116065TB</t>
   </si>
   <si>
-    <t>Saputroluki24@gmail.com</t>
+    <t>9116065TB@pln-npservices.com</t>
   </si>
   <si>
     <t>UNTUNG PRI HANDOKO</t>
@@ -374,7 +374,7 @@
     <t>9516146TB</t>
   </si>
   <si>
-    <t>Uphhandoko@gmail.com</t>
+    <t>9516146TB@pln-npservices.com</t>
   </si>
   <si>
     <t>KRISNADI SETIAWAN</t>
@@ -383,7 +383,7 @@
     <t>9317009TB</t>
   </si>
   <si>
-    <t>krisnadisetyawan212@gmail.com</t>
+    <t>9317009TB@pln-npservices.com</t>
   </si>
   <si>
     <t>ARDIANTO</t>
@@ -392,7 +392,7 @@
     <t>9416106TB</t>
   </si>
   <si>
-    <t>Bintang.ar28@gmail.com</t>
+    <t>9416106TB@pln-npservices.com</t>
   </si>
   <si>
     <t>FACHRI APRILIYAN MUTIYASNUR</t>
@@ -401,7 +401,7 @@
     <t>9716141TB</t>
   </si>
   <si>
-    <t>Fachri.apriliyan@gmail.com</t>
+    <t>9716141TB@pln-npservices.com</t>
   </si>
   <si>
     <t>AMRAN ALI</t>
@@ -410,7 +410,7 @@
     <t>9116028TB</t>
   </si>
   <si>
-    <t>amranali100891@gmail.com</t>
+    <t>9116028TB@pln-npservices.com</t>
   </si>
   <si>
     <t>NOORDIHAMSYAH MAULANAH</t>
@@ -419,7 +419,7 @@
     <t>8917010TB</t>
   </si>
   <si>
-    <t>M_maul@rocketmail.com</t>
+    <t>8917010TB@pln-npservices.com</t>
   </si>
   <si>
     <t>MUHAMMAD MAHFUD</t>
@@ -512,7 +512,7 @@
     <t>Produksi B</t>
   </si>
   <si>
-    <t>muh.irfan23@gmail.com</t>
+    <t>muh.irfan@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>APIAN DONO</t>
@@ -521,7 +521,7 @@
     <t>9016035TB</t>
   </si>
   <si>
-    <t>Apiandono@gmail.com</t>
+    <t>9016035TB@pln-npservices.com</t>
   </si>
   <si>
     <t>RANGGA DISTIANTARA</t>
@@ -530,7 +530,7 @@
     <t>9316019TB</t>
   </si>
   <si>
-    <t>Radistiantara@gmail.com &amp; dewantororanda@gmail.com</t>
+    <t>9316019TB@pln-npservices.com</t>
   </si>
   <si>
     <t>NOEGRAH TRI JULIANSYAH</t>
@@ -539,7 +539,7 @@
     <t>8916062TB</t>
   </si>
   <si>
-    <t>Noe.julian04@gmail.com</t>
+    <t>8916062TB@pln-npservices.com</t>
   </si>
   <si>
     <t>FIRMAN MAULANA HARAHAP</t>
@@ -548,7 +548,7 @@
     <t>9116094TB</t>
   </si>
   <si>
-    <t>Firmanmaulanaharahap@gmail.com</t>
+    <t>9116094TB@pln-npservices.com</t>
   </si>
   <si>
     <t>HADYAN</t>
@@ -557,7 +557,7 @@
     <t>9116029TB</t>
   </si>
   <si>
-    <t>Hadyanheixa@gmail.com</t>
+    <t>9116029TB@pln-npservices.com</t>
   </si>
   <si>
     <t>STYAWAN</t>
@@ -566,7 +566,7 @@
     <t>9116074TB</t>
   </si>
   <si>
-    <t>styawan.090791@gmail.com</t>
+    <t>9116074TB@pln-npservices.com</t>
   </si>
   <si>
     <t>RIBUT INDRAYANA</t>
@@ -575,7 +575,7 @@
     <t>9017011TB</t>
   </si>
   <si>
-    <t>Ribut862@gmail.com</t>
+    <t>9017011TB@pln-npservices.com</t>
   </si>
   <si>
     <t>MUHAMMAD ANDY</t>
@@ -584,7 +584,7 @@
     <t>9416149TB</t>
   </si>
   <si>
-    <t>Muhammadandy1994@gmail.com</t>
+    <t>9416149TB@pln-npservices.com</t>
   </si>
   <si>
     <t>HARI SUPRIANTO</t>
@@ -593,7 +593,7 @@
     <t>9416118TB</t>
   </si>
   <si>
-    <t>harysuprianto.hs@gmail.com</t>
+    <t>9416118TB@pln-npservices.com</t>
   </si>
   <si>
     <t>FERDIAN EKA PRASETYA</t>
@@ -602,7 +602,7 @@
     <t>9516134TB</t>
   </si>
   <si>
-    <t>Deianprasetya@gmail.com</t>
+    <t>9516134TB@pln-npservices.com</t>
   </si>
   <si>
     <t>ACHMAD BASOFI</t>
@@ -611,7 +611,7 @@
     <t>9417016TB</t>
   </si>
   <si>
-    <t>Basofislayer2146@gmail.com</t>
+    <t>9417016TB@pln-npservices.com</t>
   </si>
   <si>
     <t>NUR ROCHMAT</t>
@@ -620,7 +620,7 @@
     <t>9013006BR</t>
   </si>
   <si>
-    <t>Nurrochm4t@gmail.com</t>
+    <t>9013006BR@pln-npservices.com</t>
   </si>
   <si>
     <t>ACHMAD BUCHORI</t>
@@ -629,7 +629,7 @@
     <t>9716103TB</t>
   </si>
   <si>
-    <t>Achm4d.8uchori@gmail.com</t>
+    <t>9716103TB@pln-npservices.com</t>
   </si>
   <si>
     <t>JUNAID HIDAYAT</t>
@@ -638,7 +638,7 @@
     <t>9116057TB</t>
   </si>
   <si>
-    <t>Juneid1991@gmail.com</t>
+    <t>9116057TB@pln-npservices.com</t>
   </si>
   <si>
     <t>HERI SUPRIANTO</t>
@@ -722,7 +722,7 @@
     <t>Produksi C</t>
   </si>
   <si>
-    <t>Suandytison@gmail.comcom</t>
+    <t>taryono@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>FADLI</t>
@@ -731,7 +731,7 @@
     <t>9016086TB</t>
   </si>
   <si>
-    <t>El09612047@gmail.com</t>
+    <t>9016086TB@pln-npservices.com</t>
   </si>
   <si>
     <t>MUHAMMAD YUNUS</t>
@@ -740,7 +740,7 @@
     <t>9216027TB</t>
   </si>
   <si>
-    <t>muhammadyunus092@gmail.com</t>
+    <t>9216027TB@pln-npservices.com</t>
   </si>
   <si>
     <t>HARDIANSYAH</t>
@@ -749,7 +749,7 @@
     <t>9116116TB</t>
   </si>
   <si>
-    <t>Ancabahar28@gmail.com</t>
+    <t>9116116TB@pln-npservices.com</t>
   </si>
   <si>
     <t>ACHMAD FACHRIZAL</t>
@@ -758,7 +758,7 @@
     <t>9016041TB</t>
   </si>
   <si>
-    <t>Achmadfachrizal05@gmail.com</t>
+    <t>9016041TB@pln-npservices.com</t>
   </si>
   <si>
     <t>ADITYO DARMAJI</t>
@@ -767,7 +767,7 @@
     <t>9116063TB</t>
   </si>
   <si>
-    <t>Adityo.darmaji@gmail.com</t>
+    <t>9116063TB@pln-npservices.com</t>
   </si>
   <si>
     <t>HANDOKO</t>
@@ -776,7 +776,7 @@
     <t>9416052TB</t>
   </si>
   <si>
-    <t>Handokocomex@gmail.com</t>
+    <t>9416052TB@pln-npservices.com</t>
   </si>
   <si>
     <t>I WAYAN PURWANA</t>
@@ -785,7 +785,7 @@
     <t>9316087TB</t>
   </si>
   <si>
-    <t>Wayanpurwana46@gmail.com</t>
+    <t>9316087TB@pln-npservices.com</t>
   </si>
   <si>
     <t>SLAMET RIYADI</t>
@@ -794,7 +794,7 @@
     <t>8916045TB</t>
   </si>
   <si>
-    <t>Sslamet465@gmail.com</t>
+    <t>8916045TB@pln-npservices.com</t>
   </si>
   <si>
     <t>JUMARDI</t>
@@ -803,7 +803,7 @@
     <t>9516056TB</t>
   </si>
   <si>
-    <t>jumardi.adi69@gmail.com</t>
+    <t>9516056TB@pln-npservices.com</t>
   </si>
   <si>
     <t>DWI ZUNIARTO</t>
@@ -812,7 +812,7 @@
     <t>9116058TB</t>
   </si>
   <si>
-    <t>Dwizuniartoo@gmail.com</t>
+    <t>9116058TB@pln-npservices.com</t>
   </si>
   <si>
     <t>RIKI EHDHA SUBAWEH</t>
@@ -821,7 +821,7 @@
     <t>9317013TB</t>
   </si>
   <si>
-    <t>Rikiehda@gmail.com</t>
+    <t>9317013TB@pln-npservices.com</t>
   </si>
   <si>
     <t>SURYA ARMANDA</t>
@@ -830,7 +830,7 @@
     <t>9416100TB</t>
   </si>
   <si>
-    <t>Suryaarmanda39@gmail.com</t>
+    <t>9416100TB@pln-npservices.com</t>
   </si>
   <si>
     <t>BAGUS WIBOWO</t>
@@ -839,7 +839,7 @@
     <t>9116015TB</t>
   </si>
   <si>
-    <t>Baguswibowo272@yahoo.com</t>
+    <t>9116015TB@pln-npservices.com</t>
   </si>
   <si>
     <t>RACHMAD SANDY</t>
@@ -848,7 +848,7 @@
     <t>9317012TB</t>
   </si>
   <si>
-    <t>Rachmad2992@gmail.com</t>
+    <t>9317012TB@pln-npservices.com</t>
   </si>
   <si>
     <t>WISNU HABIB</t>
@@ -857,7 +857,7 @@
     <t>9516122TB</t>
   </si>
   <si>
-    <t>Wisnuhabib605@gmail.com</t>
+    <t>9516122TB@pln-npservices.com</t>
   </si>
   <si>
     <t>MUHAMMAD RANGGA CAHYADI</t>
@@ -941,7 +941,7 @@
     <t>Produksi D</t>
   </si>
   <si>
-    <t>Muhammadfauzan092@gmail.com</t>
+    <t>m.fauzan@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>GERSON YOSEP BA'KA'</t>
@@ -950,7 +950,7 @@
     <t>9116077TB</t>
   </si>
   <si>
-    <t>Gersonbaka@gmail.com</t>
+    <t>9116077TB@pln-npservices.com</t>
   </si>
   <si>
     <t>JUMADIL RAHMAN</t>
@@ -959,7 +959,7 @@
     <t>9216021TB</t>
   </si>
   <si>
-    <t>Jumadilrahman32@gmail.com</t>
+    <t>9216021TB@pln-npservices.com</t>
   </si>
   <si>
     <t>SEPTIANOER PERMADI WIBOWO</t>
@@ -968,7 +968,7 @@
     <t>9316082TB</t>
   </si>
   <si>
-    <t>Septianoer.permadi@gmail.com</t>
+    <t>9316082TB@pln-npservices.com</t>
   </si>
   <si>
     <t>MUHTAR DANI</t>
@@ -977,7 +977,7 @@
     <t>9416071TB</t>
   </si>
   <si>
-    <t>Muhtardani@gmail.com</t>
+    <t>9416071TB@pln-npservices.com</t>
   </si>
   <si>
     <t>SUGONDO PRAYOGO</t>
@@ -986,7 +986,7 @@
     <t>9216064TB</t>
   </si>
   <si>
-    <t>Sugondo06@gmail.com</t>
+    <t>9216064TB@pln-npservices.com</t>
   </si>
   <si>
     <t>MOCHAMMAD ISHAK</t>
@@ -995,7 +995,7 @@
     <t>9416079TB</t>
   </si>
   <si>
-    <t>ishakzhafran@gmail.com</t>
+    <t>9416079TB@pln-npservices.com</t>
   </si>
   <si>
     <t>AHMAD IKBAL</t>
@@ -1004,7 +1004,7 @@
     <t>9316009TB</t>
   </si>
   <si>
-    <t>Ahmadikbal93@gmail.com</t>
+    <t>9316009TB@pln-npservices.com</t>
   </si>
   <si>
     <t>DANU RACHMADDAN</t>
@@ -1013,7 +1013,7 @@
     <t>9316032TB</t>
   </si>
   <si>
-    <t>D.rachmaddan@gmail.com</t>
+    <t>9316032TB@pln-npservices.com</t>
   </si>
   <si>
     <t>HILMAN AKBAR AL HAZMI</t>
@@ -1022,7 +1022,7 @@
     <t>9316081TB</t>
   </si>
   <si>
-    <t>Hilmanalhazmi6@gmail.com</t>
+    <t>9316081TB@pln-npservices.com</t>
   </si>
   <si>
     <t>ANSHORI</t>
@@ -1031,7 +1031,7 @@
     <t>9616130TB</t>
   </si>
   <si>
-    <t>Anshoripjbs@gmail.com</t>
+    <t>9616130TB@pln-npservices.com</t>
   </si>
   <si>
     <t>FIRMAN SANTYA RUDI</t>
@@ -1040,7 +1040,7 @@
     <t>9417014TB</t>
   </si>
   <si>
-    <t>Firman.sr23@gmail.com</t>
+    <t>9417014TB@pln-npservices.com</t>
   </si>
   <si>
     <t>AUFA RAFDIKA</t>
@@ -1049,7 +1049,7 @@
     <t>8916099TB</t>
   </si>
   <si>
-    <t>Aufa.rafdika@gmail.com</t>
+    <t>8916099TB@pln-npservices.com</t>
   </si>
   <si>
     <t>AGUNG MAULANA</t>
@@ -1058,7 +1058,7 @@
     <t>9716121TB</t>
   </si>
   <si>
-    <t>maulanaagung1005@gmail.com</t>
+    <t>9716121TB@pln-npservices.com</t>
   </si>
   <si>
     <t>SETIAWAN</t>
@@ -1160,7 +1160,7 @@
     <t>Niaga &amp; Bahan Bakar</t>
   </si>
   <si>
-    <t>afik178@gmail.com</t>
+    <t>nurafiatuullah@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>AGUNG PRIA AMBARA</t>
@@ -1169,7 +1169,7 @@
     <t>9316053TB</t>
   </si>
   <si>
-    <t>Agungambara44@gmail.com</t>
+    <t>9316053TB@pln-npservices.com</t>
   </si>
   <si>
     <t>HERRY IRAWAN</t>
@@ -1178,7 +1178,7 @@
     <t>8916039TB</t>
   </si>
   <si>
-    <t>Herryirawan1988@gmail.com</t>
+    <t>8916039TB@pln-npservices.com</t>
   </si>
   <si>
     <t>NASRUL</t>
@@ -1208,7 +1208,7 @@
     <t>Kimia</t>
   </si>
   <si>
-    <t>mudzofars@gmail.com</t>
+    <t>mudzofar.sofyan@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>ANDHIKA</t>
@@ -1217,7 +1217,7 @@
     <t>9316108TB</t>
   </si>
   <si>
-    <t>Dhikayoo@gmail.com</t>
+    <t>9316108TB@pln-npservices.com</t>
   </si>
   <si>
     <t>MIFTAKHUL HUDA</t>
@@ -1226,7 +1226,7 @@
     <t>9216038TB</t>
   </si>
   <si>
-    <t>Mifta.huda07@gmail.com</t>
+    <t>9216038TB@pln-npservices.com</t>
   </si>
   <si>
     <t>REZA IBNU MULIA</t>
@@ -1235,7 +1235,7 @@
     <t>9316023TB</t>
   </si>
   <si>
-    <t>rezaibnu@ymail.com &amp; laborujkt@gmail.com</t>
+    <t>9316023TB@pln-npservices.com</t>
   </si>
   <si>
     <t>ENDI PRASETIO</t>
@@ -1301,7 +1301,7 @@
     <t>Pemeliharaan</t>
   </si>
   <si>
-    <t>misdipjb@gmail.com</t>
+    <t>misdiyanto@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>NASRI MATHAR</t>
@@ -1313,7 +1313,7 @@
     <t>Rendal Pemeliharaan</t>
   </si>
   <si>
-    <t>nazrimathar@gmail.com</t>
+    <t>nasri.mathar@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>BANGKIT INDRA PRATAMA</t>
@@ -1322,7 +1322,7 @@
     <t>9116017TB</t>
   </si>
   <si>
-    <t>Bangkitindrap@gmail.com</t>
+    <t>9116017TB@pln-npservices.com</t>
   </si>
   <si>
     <t>FAJRIN ZAINUDDIN</t>
@@ -1331,7 +1331,7 @@
     <t>9016075TB</t>
   </si>
   <si>
-    <t>Fajrinzain10@gmail.com</t>
+    <t>9016075TB@pln-npservices.com</t>
   </si>
   <si>
     <t>MUHAMMAD ARGHU</t>
@@ -1340,7 +1340,7 @@
     <t>9416150TB</t>
   </si>
   <si>
-    <t>Muh.arghu@gmail.com</t>
+    <t>9416150TB@pln-npservices.com</t>
   </si>
   <si>
     <t>SURIANTO</t>
@@ -1349,7 +1349,7 @@
     <t>9317007TB</t>
   </si>
   <si>
-    <t>surianto.sk@gmail.com</t>
+    <t>9317007TB@pln-npservices.com</t>
   </si>
   <si>
     <t>RUDY SETYANA RAHARJO</t>
@@ -1358,7 +1358,7 @@
     <t>8916078TB</t>
   </si>
   <si>
-    <t>rudyruudrush@gmail.com</t>
+    <t>8916078TB@pln-npservices.com</t>
   </si>
   <si>
     <t>KHRIS DIANTO TOMBOKAN</t>
@@ -1388,7 +1388,7 @@
     <t>Outage Management</t>
   </si>
   <si>
-    <t>tonykediri87@gmail.com</t>
+    <t>tony.suharto@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>MAYKY ARISDA SUMANTO</t>
@@ -1397,7 +1397,7 @@
     <t>8715008TD</t>
   </si>
   <si>
-    <t>max8715008td@gmail.com</t>
+    <t>8715008TD@pln-npservices.com</t>
   </si>
   <si>
     <t>MUHAMMAD ADITYAWARMAN</t>
@@ -1406,7 +1406,7 @@
     <t>9116044PL</t>
   </si>
   <si>
-    <t>Adiwarman05@gmail.com</t>
+    <t>9116044PL@pln-npservices.com</t>
   </si>
   <si>
     <t>FAHMI HERMAWAN</t>
@@ -1415,7 +1415,7 @@
     <t>9116137TB</t>
   </si>
   <si>
-    <t>Fahmihermawan8@gmail.com</t>
+    <t>9116137TB@pln-npservices.com</t>
   </si>
   <si>
     <t>DWI PRANOTO</t>
@@ -1436,7 +1436,7 @@
     <t>Pemeliharaan Mesin 1 B, T &amp; AAB</t>
   </si>
   <si>
-    <t>nave.satria@gmail.com</t>
+    <t>evan.satria@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>HERI SISWANTO</t>
@@ -1445,7 +1445,7 @@
     <t>9116095TB</t>
   </si>
   <si>
-    <t>herisiswanto8@gmail.com</t>
+    <t>9116095TB@pln-npservices.com</t>
   </si>
   <si>
     <t>INDRA SAPUTRA SIAHAAN</t>
@@ -1454,7 +1454,7 @@
     <t>9416089TB</t>
   </si>
   <si>
-    <t>Indrakrezen2@gmail.com</t>
+    <t>9416089TB@pln-npservices.com</t>
   </si>
   <si>
     <t>TRI SUPRIADI</t>
@@ -1463,7 +1463,7 @@
     <t>9217008TB</t>
   </si>
   <si>
-    <t>Iamtriee@gmail.com</t>
+    <t>9217008TB@pln-npservices.com</t>
   </si>
   <si>
     <t>EDI TIARDI</t>
@@ -1472,7 +1472,7 @@
     <t>9316151TB</t>
   </si>
   <si>
-    <t>Editiardi25@gmail.com</t>
+    <t>9316151TB@pln-npservices.com</t>
   </si>
   <si>
     <t>JUHAMSYARIE</t>
@@ -1481,7 +1481,7 @@
     <t>9416144TB</t>
   </si>
   <si>
-    <t>Juhamsyarie@gmail.com</t>
+    <t>9416144TB@pln-npservices.com</t>
   </si>
   <si>
     <t>KHAIRUL ARIFIN PANGGE</t>
@@ -1490,7 +1490,7 @@
     <t>9716135TB</t>
   </si>
   <si>
-    <t>Khairularifin927@gmail.com</t>
+    <t>9716135TB@pln-npservices.com</t>
   </si>
   <si>
     <t>MARIANSYAH</t>
@@ -1499,7 +1499,7 @@
     <t>9516145TB</t>
   </si>
   <si>
-    <t>Mariansyahreal14@gmail.com</t>
+    <t>9516145TB@pln-npservices.com</t>
   </si>
   <si>
     <t>MUHAMAD ICHSANUDIN</t>
@@ -1508,7 +1508,7 @@
     <t>9316109TB</t>
   </si>
   <si>
-    <t>Ihsandhafa@gmail.com</t>
+    <t>9316109TB@pln-npservices.com</t>
   </si>
   <si>
     <t>MUHAMMAD JAYA MAYYASA</t>
@@ -1517,7 +1517,7 @@
     <t>9616140TB</t>
   </si>
   <si>
-    <t>M.jayamayyasa96@gmail.com</t>
+    <t>9616140TB@pln-npservices.com</t>
   </si>
   <si>
     <t>SUTIKNO</t>
@@ -1664,7 +1664,7 @@
     <t>Pemeliharaan Mesin 2 &amp; Sipil</t>
   </si>
   <si>
-    <t>kholik.khusnul@gmail.com</t>
+    <t>9016097TB@pln-npservices.com</t>
   </si>
   <si>
     <t>TAUFIK AFRIANDY NAPITUPULU</t>
@@ -1673,7 +1673,7 @@
     <t>9016098TB</t>
   </si>
   <si>
-    <t>taufik.an670@gmail.com</t>
+    <t>9016098TB@pln-npservices.com</t>
   </si>
   <si>
     <t>EDY NURDIANSYAH</t>
@@ -1682,7 +1682,7 @@
     <t>9516136TB</t>
   </si>
   <si>
-    <t>Edy.knox@gmail.com</t>
+    <t>9516136TB@pln-npservices.com</t>
   </si>
   <si>
     <t>IKHSAN PRAYOGI</t>
@@ -1691,7 +1691,7 @@
     <t>9416148TB</t>
   </si>
   <si>
-    <t>Ikhsanprayoogi@gmail.com</t>
+    <t>9416148TB@pln-npservices.com</t>
   </si>
   <si>
     <t>KAMAL HASAN</t>
@@ -1700,7 +1700,7 @@
     <t>9616142TB</t>
   </si>
   <si>
-    <t>Kamahasanojt8@gmail.com</t>
+    <t>9616142TB@pln-npservices.com</t>
   </si>
   <si>
     <t>REZA AZHARI</t>
@@ -1709,7 +1709,7 @@
     <t>8817074PL</t>
   </si>
   <si>
-    <t>Azharireza88@gmail.com</t>
+    <t>8817074PL@pln-npservices.com</t>
   </si>
   <si>
     <t>JULI PAJAR WALOYO</t>
@@ -1718,7 +1718,7 @@
     <t>8913001BR</t>
   </si>
   <si>
-    <t>jullypjr@gmail.com</t>
+    <t>8913001BR@pln-npservices.com</t>
   </si>
   <si>
     <t>ROBERT SIRANDA</t>
@@ -1883,7 +1883,7 @@
     <t>Pemeliharaan Listrik</t>
   </si>
   <si>
-    <t>faqihxalfaruq@gmail.com</t>
+    <t>faqih.alfaruq@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>MUHAMMAD MUSTAFA</t>
@@ -1892,7 +1892,7 @@
     <t>9316073TB</t>
   </si>
   <si>
-    <t>mustafamuhammad866@gmail.com</t>
+    <t>9316073TB@pln-npservices.com</t>
   </si>
   <si>
     <t>PERRY BURA</t>
@@ -1901,7 +1901,7 @@
     <t>8916037TB</t>
   </si>
   <si>
-    <t>Perrybura17@gmail.com</t>
+    <t>8916037TB@pln-npservices.com</t>
   </si>
   <si>
     <t>REZA PRATAMA</t>
@@ -1910,7 +1910,7 @@
     <t>9416084TB</t>
   </si>
   <si>
-    <t>Reza.pratama27@gmail.com</t>
+    <t>9416084TB@pln-npservices.com</t>
   </si>
   <si>
     <t>YOGI PRATAMA</t>
@@ -1919,7 +1919,7 @@
     <t>9316011TB</t>
   </si>
   <si>
-    <t>Yogipratama164@gmail.com</t>
+    <t>9316011TB@pln-npservices.com</t>
   </si>
   <si>
     <t>OXSA ANUGRAH</t>
@@ -1928,7 +1928,7 @@
     <t>9716128TB</t>
   </si>
   <si>
-    <t>Anugrahoxsa@gmail.com</t>
+    <t>9716128TB@pln-npservices.com</t>
   </si>
   <si>
     <t>MUHAMMAD HASBI</t>
@@ -1937,7 +1937,7 @@
     <t>9216043TB</t>
   </si>
   <si>
-    <t>Hasbi1717@yahoo.com</t>
+    <t>9216043TB@pln-npservices.com</t>
   </si>
   <si>
     <t>CHANDRA DWI SAPUTRA</t>
@@ -1946,7 +1946,7 @@
     <t>9516125TB</t>
   </si>
   <si>
-    <t>Candramickey@gmail.com</t>
+    <t>9516125TB@pln-npservices.com</t>
   </si>
   <si>
     <t>ADI PRAMONO</t>
@@ -2039,7 +2039,7 @@
     <t>Pemeliharaan Kontrol &amp; Instrumen</t>
   </si>
   <si>
-    <t>Rimmer.kaltim@gmail.com</t>
+    <t>rimmer@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>DANANG PRASETYA</t>
@@ -2048,7 +2048,7 @@
     <t>9416080TB</t>
   </si>
   <si>
-    <t>Danangdasilva@gmail.com</t>
+    <t>9416080TB@pln-npservices.com</t>
   </si>
   <si>
     <t>RISZKI WAHYU ADINATA</t>
@@ -2057,7 +2057,7 @@
     <t>9416083TB</t>
   </si>
   <si>
-    <t>Riszkiw@gmail.com</t>
+    <t>9416083TB@pln-npservices.com</t>
   </si>
   <si>
     <t>ANGGA ARRYANDA PUTRA HIDAYAT</t>
@@ -2066,7 +2066,7 @@
     <t>9516123TB</t>
   </si>
   <si>
-    <t>Anggaryandha176@gmail.com</t>
+    <t>9516123TB@pln-npservices.com</t>
   </si>
   <si>
     <t>BAYU PRASETYO</t>
@@ -2075,7 +2075,7 @@
     <t>9716133TB</t>
   </si>
   <si>
-    <t>Bayu.prasetyo441@gmail.com</t>
+    <t>9716133TB@pln-npservices.com</t>
   </si>
   <si>
     <t>JAKA WENDIS EKA SAPUTRA</t>
@@ -2084,7 +2084,7 @@
     <t>9516059TB</t>
   </si>
   <si>
-    <t>Jakawendis.es@gmail.com</t>
+    <t>9516059TB@pln-npservices.com</t>
   </si>
   <si>
     <t>NAUFAL RIZKI SYAPUTRA</t>
@@ -2093,7 +2093,7 @@
     <t>9716127TB</t>
   </si>
   <si>
-    <t>Opexgood@gmail.com</t>
+    <t>9716127TB@pln-npservices.com</t>
   </si>
   <si>
     <t>ZUQNI SEPTIAN</t>
@@ -2102,7 +2102,7 @@
     <t>9316153TB</t>
   </si>
   <si>
-    <t>Zukni.septian@gmail.com</t>
+    <t>9316153TB@pln-npservices.com</t>
   </si>
   <si>
     <t>ADJI NURHIDDAYAT</t>
@@ -2186,7 +2186,7 @@
     <t>Inventori Kontrol &amp; Gudang</t>
   </si>
   <si>
-    <t>awan.jirolu@gmail.com</t>
+    <t>wawan.hendri@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>IKWAL IDUL FIKRI</t>
@@ -2195,7 +2195,7 @@
     <t>9116024TB</t>
   </si>
   <si>
-    <t>Ikwal.fikri@pjbs.com</t>
+    <t>9116024tb@pln-npservices.com</t>
   </si>
   <si>
     <t>WISNU DWI YANTO</t>
@@ -2204,7 +2204,7 @@
     <t>9616104TB</t>
   </si>
   <si>
-    <t>Wisnudwiy66@gmail.com &amp; wisnuastrisena@gmail.com</t>
+    <t>9616104TB@pln-npservices.com</t>
   </si>
   <si>
     <t>YULIO DESTA FEBRIONA HIDAYATI</t>
@@ -2213,7 +2213,7 @@
     <t>9516105TB</t>
   </si>
   <si>
-    <t>yuliodesta321@gmail.com</t>
+    <t>9516105TB@pln-npservices.com</t>
   </si>
   <si>
     <t>AHMAD CHOERUL SAHRI</t>
@@ -2222,7 +2222,7 @@
     <t>8913032BR</t>
   </si>
   <si>
-    <t>Ahmadchoerul89@gmail.com</t>
+    <t>8913032BR@pln-npservices.com</t>
   </si>
   <si>
     <t>SURYA PERDANA</t>
@@ -2231,7 +2231,7 @@
     <t>9416042TB</t>
   </si>
   <si>
-    <t>suryaperdana425@gmail.com</t>
+    <t>9416042TB@pln-npservices.com</t>
   </si>
   <si>
     <t>RIKARDONIUS TUMANGGOR</t>
@@ -2261,7 +2261,7 @@
     <t>Enjiniring &amp; Quality Assurance</t>
   </si>
   <si>
-    <t>azr_tm02@yahoo.com</t>
+    <t>muhammad.arif@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>GUSTI PRYANDARU</t>
@@ -2273,7 +2273,7 @@
     <t>Condition Based Maintenance</t>
   </si>
   <si>
-    <t>gustipryandaru@gmail.com</t>
+    <t>gusti.pryandaru@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>RICARDO</t>
@@ -2282,7 +2282,7 @@
     <t>9216034TB</t>
   </si>
   <si>
-    <t>Ricardokbmk@gmail.com</t>
+    <t>9216034TB@pln-npservices.com</t>
   </si>
   <si>
     <t>RISKO RAHMAN NOOR</t>
@@ -2291,7 +2291,7 @@
     <t>9316012TB</t>
   </si>
   <si>
-    <t>riskorahman93@gmail.com</t>
+    <t>9316012TB@pln-npservices.com</t>
   </si>
   <si>
     <t>SENO SATRIA</t>
@@ -2321,7 +2321,7 @@
     <t>System Owner</t>
   </si>
   <si>
-    <t>anugrah.janardana@gmail.com</t>
+    <t>gede.bayu@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>ARBIAN TRIHARTONO</t>
@@ -2330,7 +2330,7 @@
     <t>9016018TB</t>
   </si>
   <si>
-    <t>Arbian.trihartono@gmail.com</t>
+    <t>arbian.tri@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>AGUSTIAN RAHMAT</t>
@@ -2339,7 +2339,7 @@
     <t>9116049TB</t>
   </si>
   <si>
-    <t>Agutirrah@gmail.com</t>
+    <t>9116049TB@pln-npservices.com</t>
   </si>
   <si>
     <t>AGUNG WIJAYANTO</t>
@@ -2348,7 +2348,7 @@
     <t>9217073PL</t>
   </si>
   <si>
-    <t>agungwwijayanto@outlook.com / Xagungwijayantox@gmail.com</t>
+    <t>9217073PL@pln-npservices.com</t>
   </si>
   <si>
     <t>FRANKY NOPRYANTO</t>
@@ -2357,7 +2357,7 @@
     <t>8916007TB</t>
   </si>
   <si>
-    <t>Frankienoprianto@gmail.com</t>
+    <t>8916007TB@pln-npservices.com</t>
   </si>
   <si>
     <t>DAVID HERMAWAN</t>
@@ -2366,7 +2366,7 @@
     <t>9316025TB</t>
   </si>
   <si>
-    <t>davidhermawan122@gmail.com</t>
+    <t>9316025TB@pln-npservices.com</t>
   </si>
   <si>
     <t>MUHAMMAD AN NUUR ISLAM</t>
@@ -2375,7 +2375,7 @@
     <t>9316016TB</t>
   </si>
   <si>
-    <t>annoer.respect365@gmail.com</t>
+    <t>9316016TB@pln-npservices.com</t>
   </si>
   <si>
     <t>DWI PUJIANTO</t>
@@ -2384,7 +2384,7 @@
     <t>9216124TB</t>
   </si>
   <si>
-    <t>Dwi.pujianto27@gmail.com</t>
+    <t>9216124TB@pln-npservices.com</t>
   </si>
   <si>
     <t>DEDDY IRAWAN</t>
@@ -2405,7 +2405,7 @@
     <t>Manajemen Mutu Risiko &amp; Kepatuhan</t>
   </si>
   <si>
-    <t>agistarizky@gmail.com</t>
+    <t>agista.rizky@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>MUHAMMAD ANZAR</t>
@@ -2414,7 +2414,7 @@
     <t>9316131TB</t>
   </si>
   <si>
-    <t>Anzargavigun@gmail.com</t>
+    <t>9316131TB@pln-npservices.com</t>
   </si>
   <si>
     <t>TEGUH DWI SUSANTO</t>
@@ -2423,7 +2423,7 @@
     <t>9116013TB</t>
   </si>
   <si>
-    <t>teguhsusanto420@gmail.com</t>
+    <t>9116013TB@pln-npservices.com</t>
   </si>
   <si>
     <t>SANDI WIDYANTO</t>
@@ -2432,7 +2432,7 @@
     <t>8816076TB</t>
   </si>
   <si>
-    <t>Sandiwidyanto@gmail.com</t>
+    <t>8816076TB@pln-npservices.com</t>
   </si>
   <si>
     <t>WAHYU BUDI DHARMAWAN</t>
@@ -2456,7 +2456,7 @@
     <t>Keuangan</t>
   </si>
   <si>
-    <t>adilo.aristo@gmail.com</t>
+    <t>aristo.titis@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>NINDIA TYASING KUSUMAWARDANI</t>
@@ -2495,7 +2495,7 @@
     <t>SDM, Umum &amp; CSR</t>
   </si>
   <si>
-    <t>bambangbagja@gmail.com</t>
+    <t>bambang.bagja@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>ERMA YUNITA</t>
@@ -2504,7 +2504,7 @@
     <t>9116114TB</t>
   </si>
   <si>
-    <t>Tata.sitata92@gmail.com</t>
+    <t>9116114TB@pln-npservices.com</t>
   </si>
   <si>
     <t>MUHAMMAD ARSYAD</t>
@@ -2513,7 +2513,7 @@
     <t>9216111TB</t>
   </si>
   <si>
-    <t>Arsyadmsp@gmail.com</t>
+    <t>9216111TB@pln-npservices.com</t>
   </si>
   <si>
     <t>NUR HIDAYAH</t>
@@ -2531,7 +2531,7 @@
     <t>9516072PL</t>
   </si>
   <si>
-    <t>yudatanex@gmail.com</t>
+    <t>9516072PL@pln-npservices.com</t>
   </si>
   <si>
     <t>RIZA MEIRISAH</t>
@@ -2540,7 +2540,7 @@
     <t>9416102TB</t>
   </si>
   <si>
-    <t>Rizameirisah@gmail.com</t>
+    <t>9416102TB@pln-npservices.com</t>
   </si>
   <si>
     <t>LUTHFI ABDUL GHONI</t>
@@ -2570,7 +2570,7 @@
     <t>Pengadaan</t>
   </si>
   <si>
-    <t>dzikri.irhami@gmail.com</t>
+    <t>dzikri@plnnusantarapower.co.id</t>
   </si>
   <si>
     <t>WISDOMI WASIH S PURBA</t>
@@ -2579,7 +2579,7 @@
     <t>8715005TB</t>
   </si>
   <si>
-    <t>Wisdomiwsp@gmail.com</t>
+    <t>8715005TB@pln-npservices.com</t>
   </si>
   <si>
     <t>IKE LUVITA AYUNANI</t>
@@ -2588,7 +2588,7 @@
     <t>9117043PL</t>
   </si>
   <si>
-    <t>Ikeluvita91@gmail.com</t>
+    <t>9117043PL@pln-npservices.com</t>
   </si>
   <si>
     <t>ELISABETH</t>
@@ -2636,7 +2636,7 @@
     <t>9317002RP</t>
   </si>
   <si>
-    <t>r.nurroyyan@gmail.com</t>
+    <t>9317002RP@pln-npservices.com</t>
   </si>
 </sst>
 </file>
@@ -3830,7 +3830,7 @@
   <dimension ref="A2:E281"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E281" sqref="E281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -8606,7 +8606,7 @@
   <hyperlinks>
     <hyperlink ref="E272" r:id="rId1" display="Agluthfi21@gmail.com"/>
     <hyperlink ref="E261" r:id="rId2" display="wahyubudi@plnnusantarapower.co.id" tooltip="mailto:wahyubudi@plnnusantarapower.co.id"/>
-    <hyperlink ref="E123" r:id="rId3" display="afik178@gmail.com"/>
+    <hyperlink ref="E123" r:id="rId3" display="nurafiatuullah@plnnusantarapower.co.id"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>